<commit_message>
fixing ids attribute bumping version
</commit_message>
<xml_diff>
--- a/ad_works/pipelines/tables.xlsx
+++ b/ad_works/pipelines/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/databricks-patterns/ad_works/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7E7BB-52FC-B94A-9D40-A97E5FFD3638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A1B36C-90AE-C040-A55A-0263BBB1F1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>table</t>
   </si>
   <si>
-    <t>ids</t>
-  </si>
-  <si>
     <t>depends_on</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>raw</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
   <si>
     <t>rentention_days</t>
@@ -1248,9 +1248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}">
   <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,10 +1299,10 @@
         <v>22</v>
       </c>
       <c r="F1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>5</v>
       </c>
       <c r="H1" s="22" t="s">
         <v>26</v>
@@ -1313,19 +1313,19 @@
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
       <c r="N1" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="19"/>
       <c r="R1" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
       <c r="U1" s="18"/>
       <c r="V1" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W1" s="23"/>
     </row>
@@ -1356,31 +1356,31 @@
         <v>30</v>
       </c>
       <c r="N2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="R2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="W2" s="13" t="s">
         <v>20</v>
@@ -1388,16 +1388,16 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>23</v>
@@ -1428,10 +1428,10 @@
     </row>
     <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="5" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>33</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>33</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>33</v>
@@ -1513,10 +1513,10 @@
     </row>
     <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>33</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>33</v>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>33</v>
@@ -1555,10 +1555,10 @@
     </row>
     <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>33</v>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>33</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>33</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>33</v>
@@ -1611,10 +1611,10 @@
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
@@ -1625,10 +1625,10 @@
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>33</v>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>33</v>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>33</v>
@@ -1667,10 +1667,10 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>33</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>33</v>
@@ -1695,10 +1695,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>33</v>
@@ -1709,10 +1709,10 @@
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>33</v>
@@ -1723,10 +1723,10 @@
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>33</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>33</v>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>33</v>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>33</v>
@@ -1793,10 +1793,10 @@
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>33</v>
@@ -1807,10 +1807,10 @@
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>33</v>
@@ -1821,10 +1821,10 @@
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>33</v>
@@ -1835,10 +1835,10 @@
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>33</v>
@@ -1849,10 +1849,10 @@
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>33</v>
@@ -1863,10 +1863,10 @@
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>33</v>
@@ -1877,10 +1877,10 @@
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>33</v>
@@ -1891,10 +1891,10 @@
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>33</v>
@@ -1905,10 +1905,10 @@
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>33</v>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>33</v>
@@ -1933,10 +1933,10 @@
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>33</v>
@@ -1947,10 +1947,10 @@
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>33</v>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>33</v>
@@ -1975,10 +1975,10 @@
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>33</v>
@@ -1989,10 +1989,10 @@
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>33</v>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>33</v>
@@ -2017,10 +2017,10 @@
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>33</v>
@@ -2031,10 +2031,10 @@
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>33</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>33</v>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>33</v>
@@ -2073,10 +2073,10 @@
     </row>
     <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>33</v>
@@ -2087,10 +2087,10 @@
     </row>
     <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>33</v>
@@ -2101,10 +2101,10 @@
     </row>
     <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>33</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>33</v>
@@ -2129,10 +2129,10 @@
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>33</v>
@@ -2143,10 +2143,10 @@
     </row>
     <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>33</v>
@@ -2157,10 +2157,10 @@
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>33</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>33</v>
@@ -2185,10 +2185,10 @@
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>33</v>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>33</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>33</v>
@@ -2227,10 +2227,10 @@
     </row>
     <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>33</v>
@@ -2241,10 +2241,10 @@
     </row>
     <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>33</v>
@@ -2255,10 +2255,10 @@
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>33</v>
@@ -2269,10 +2269,10 @@
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>33</v>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="65" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>33</v>
@@ -2297,10 +2297,10 @@
     </row>
     <row r="66" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>33</v>
@@ -2311,10 +2311,10 @@
     </row>
     <row r="67" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>33</v>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="68" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>33</v>
@@ -2339,10 +2339,10 @@
     </row>
     <row r="69" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>33</v>
@@ -2353,10 +2353,10 @@
     </row>
     <row r="70" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>33</v>
@@ -2367,10 +2367,10 @@
     </row>
     <row r="71" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>33</v>
@@ -2383,10 +2383,10 @@
     </row>
     <row r="72" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>35</v>
@@ -2421,10 +2421,10 @@
     </row>
     <row r="73" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>35</v>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="74" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>35</v>
@@ -2497,10 +2497,10 @@
     </row>
     <row r="75" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>35</v>
@@ -2535,10 +2535,10 @@
     </row>
     <row r="76" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>35</v>
@@ -2573,10 +2573,10 @@
     </row>
     <row r="77" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>35</v>
@@ -2611,10 +2611,10 @@
     </row>
     <row r="78" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>35</v>
@@ -2649,10 +2649,10 @@
     </row>
     <row r="79" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>35</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="80" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>35</v>
@@ -2725,10 +2725,10 @@
     </row>
     <row r="81" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>35</v>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="82" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>35</v>
@@ -2801,10 +2801,10 @@
     </row>
     <row r="83" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>35</v>
@@ -2839,10 +2839,10 @@
     </row>
     <row r="84" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>35</v>
@@ -2877,10 +2877,10 @@
     </row>
     <row r="85" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>35</v>
@@ -2915,10 +2915,10 @@
     </row>
     <row r="86" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>35</v>
@@ -2953,10 +2953,10 @@
     </row>
     <row r="87" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>35</v>
@@ -2991,10 +2991,10 @@
     </row>
     <row r="88" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>35</v>
@@ -3029,10 +3029,10 @@
     </row>
     <row r="89" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>35</v>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="90" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>35</v>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="91" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>35</v>
@@ -3143,10 +3143,10 @@
     </row>
     <row r="92" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>35</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="93" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>35</v>
@@ -3219,10 +3219,10 @@
     </row>
     <row r="94" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>35</v>
@@ -3257,10 +3257,10 @@
     </row>
     <row r="95" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>35</v>
@@ -3293,10 +3293,10 @@
     </row>
     <row r="96" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>35</v>
@@ -3331,10 +3331,10 @@
     </row>
     <row r="97" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>35</v>
@@ -3369,10 +3369,10 @@
     </row>
     <row r="98" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>35</v>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="99" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>35</v>
@@ -3445,10 +3445,10 @@
     </row>
     <row r="100" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>35</v>
@@ -3483,10 +3483,10 @@
     </row>
     <row r="101" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>35</v>
@@ -3521,10 +3521,10 @@
     </row>
     <row r="102" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>35</v>
@@ -3559,10 +3559,10 @@
     </row>
     <row r="103" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>35</v>
@@ -3597,10 +3597,10 @@
     </row>
     <row r="104" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>35</v>
@@ -3635,10 +3635,10 @@
     </row>
     <row r="105" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>35</v>
@@ -3673,10 +3673,10 @@
     </row>
     <row r="106" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>35</v>
@@ -3711,10 +3711,10 @@
     </row>
     <row r="107" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>35</v>
@@ -3749,10 +3749,10 @@
     </row>
     <row r="108" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>35</v>
@@ -3787,10 +3787,10 @@
     </row>
     <row r="109" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>35</v>
@@ -3825,10 +3825,10 @@
     </row>
     <row r="110" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>35</v>
@@ -3863,10 +3863,10 @@
     </row>
     <row r="111" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>35</v>
@@ -3901,10 +3901,10 @@
     </row>
     <row r="112" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>35</v>
@@ -3939,10 +3939,10 @@
     </row>
     <row r="113" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>35</v>
@@ -3977,10 +3977,10 @@
     </row>
     <row r="114" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>35</v>
@@ -4015,10 +4015,10 @@
     </row>
     <row r="115" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>35</v>
@@ -4053,10 +4053,10 @@
     </row>
     <row r="116" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>35</v>
@@ -4091,10 +4091,10 @@
     </row>
     <row r="117" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>35</v>
@@ -4129,10 +4129,10 @@
     </row>
     <row r="118" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>35</v>
@@ -4167,10 +4167,10 @@
     </row>
     <row r="119" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>35</v>
@@ -4205,10 +4205,10 @@
     </row>
     <row r="120" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>35</v>
@@ -4243,10 +4243,10 @@
     </row>
     <row r="121" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>35</v>
@@ -4281,10 +4281,10 @@
     </row>
     <row r="122" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>35</v>
@@ -4319,10 +4319,10 @@
     </row>
     <row r="123" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>35</v>
@@ -4357,10 +4357,10 @@
     </row>
     <row r="124" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>35</v>
@@ -4395,10 +4395,10 @@
     </row>
     <row r="125" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>35</v>
@@ -4433,10 +4433,10 @@
     </row>
     <row r="126" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>35</v>
@@ -4471,10 +4471,10 @@
     </row>
     <row r="127" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>35</v>
@@ -4509,10 +4509,10 @@
     </row>
     <row r="128" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>35</v>
@@ -4547,10 +4547,10 @@
     </row>
     <row r="129" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>35</v>
@@ -4585,10 +4585,10 @@
     </row>
     <row r="130" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>35</v>
@@ -4623,10 +4623,10 @@
     </row>
     <row r="131" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>35</v>
@@ -4661,10 +4661,10 @@
     </row>
     <row r="132" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>35</v>
@@ -4699,10 +4699,10 @@
     </row>
     <row r="133" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>35</v>
@@ -4737,10 +4737,10 @@
     </row>
     <row r="134" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>35</v>
@@ -4775,10 +4775,10 @@
     </row>
     <row r="135" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>35</v>
@@ -4813,10 +4813,10 @@
     </row>
     <row r="136" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>35</v>
@@ -4851,10 +4851,10 @@
     </row>
     <row r="137" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>35</v>
@@ -4889,10 +4889,10 @@
     </row>
     <row r="138" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>35</v>
@@ -4927,10 +4927,10 @@
     </row>
     <row r="139" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
reconfigure  ad works dw
</commit_message>
<xml_diff>
--- a/ad_works/pipelines/tables.xlsx
+++ b/ad_works/pipelines/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunryan/databricks-patterns/ad_works/pipelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083479F0-F264-7D45-8441-5E64C2C15004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ECBC7F-AA0E-3C4D-9A26-586839C4C121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF8CC655-0BC7-D149-95AE-B93FEDAFD6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,18 +137,6 @@
     <t>production_product_model_product_description_culture</t>
   </si>
   <si>
-    <t>landing_ad_works</t>
-  </si>
-  <si>
-    <t>raw.raw_ad_works.*</t>
-  </si>
-  <si>
-    <t>raw_ad_works</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_model_product_description_culture</t>
-  </si>
-  <si>
     <t>hr_department</t>
   </si>
   <si>
@@ -332,186 +320,6 @@
     <t>sales_store</t>
   </si>
   <si>
-    <t>landing.landing_ad_works.hr_department</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.hr_employee</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.hr_employee_department_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.hr_employee_pay_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.hr_job_candidate</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.hr_shift</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_address</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_address_type</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_business_entity</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_business_entity_address</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_business_entity_contact</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_contact_type</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_country_region</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_email_address</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_password</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_person</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_personp_phone</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_phone_number_type</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.person_state_province</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_bill_of_materials</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_culture</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_document</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_illustration</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_location</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_category</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_cost_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_description</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_document</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_inventory</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_list_price_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_model</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_model_illustration</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_photo</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_product_photo</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_review</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_product_subcategory</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_scrap_reason</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_transaction_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_transaction_history_archive</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_unit_measure</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_country_region_currency</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_credit_card</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_currency</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_currency_rate</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_customer</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_person_credit_card</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_order_detail</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_order_header</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_order_header_sales_reason</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_person</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_person_quota_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_reason</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_tax_rate</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_territory</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_sales_territory_history</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_shopping_cart_item</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_special_offer</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_special_offer_product</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.sales_store</t>
-  </si>
-  <si>
     <t>production_work_order_routing</t>
   </si>
   <si>
@@ -528,27 +336,6 @@
   </si>
   <si>
     <t>purchasing_vendor</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_work_order</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.production_work_order_routing</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.purchasing_product_vendor</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.purchasing_purchase_order_detail</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.purchasing_purchase_order_header</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.purchasing_ship_method</t>
-  </si>
-  <si>
-    <t>landing.landing_ad_works.purchasing_vendor</t>
   </si>
   <si>
     <t>production_work_order</t>
@@ -757,7 +544,220 @@
 ProductID</t>
   </si>
   <si>
-    <t>control_ad_works</t>
+    <t>yetl_control_ad_works</t>
+  </si>
+  <si>
+    <t>yetl_landing_ad_works</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.hr_department</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.hr_employee</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.hr_employee_department_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.hr_employee_pay_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.hr_job_candidate</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.hr_shift</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_address</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_address_type</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_business_entity</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_business_entity_address</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_business_entity_contact</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_contact_type</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_country_region</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_email_address</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_password</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_person</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_personp_phone</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_phone_number_type</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.person_state_province</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_bill_of_materials</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_culture</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_document</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_illustration</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_location</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_category</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_cost_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_description</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_document</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_inventory</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_list_price_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_model</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_model_illustration</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_model_product_description_culture</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_photo</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_product_photo</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_review</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_product_subcategory</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_scrap_reason</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_transaction_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_transaction_history_archive</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_unit_measure</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_work_order</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.production_work_order_routing</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.purchasing_product_vendor</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.purchasing_purchase_order_detail</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.purchasing_purchase_order_header</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.purchasing_ship_method</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.purchasing_vendor</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_country_region_currency</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_credit_card</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_currency</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_currency_rate</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_customer</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_person_credit_card</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_order_detail</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_order_header</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_order_header_sales_reason</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_person</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_person_quota_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_reason</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_tax_rate</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_territory</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_sales_territory_history</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_shopping_cart_item</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_special_offer</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_special_offer_product</t>
+  </si>
+  <si>
+    <t>landing.yetl_landing_ad_works.sales_store</t>
+  </si>
+  <si>
+    <t>raw.yetl_raw_ad_works.*</t>
+  </si>
+  <si>
+    <t>yetl_raw_ad_works</t>
   </si>
 </sst>
 </file>
@@ -915,16 +915,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1250,7 +1250,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1283,25 +1283,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="25" t="s">
@@ -1312,31 +1312,31 @@
       <c r="K1" s="25"/>
       <c r="L1" s="25"/>
       <c r="M1" s="25"/>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="23" t="s">
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
       <c r="V1" s="26" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="26"/>
     </row>
     <row r="2" spans="1:24" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>33</v>
+        <v>228</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1434,10 +1434,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1449,10 +1449,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1463,10 +1463,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1477,10 +1477,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1491,10 +1491,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1505,10 +1505,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1519,10 +1519,10 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1533,10 +1533,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1547,10 +1547,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1561,10 +1561,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1575,10 +1575,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1589,10 +1589,10 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1603,10 +1603,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1617,10 +1617,10 @@
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1631,10 +1631,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1645,10 +1645,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1659,10 +1659,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1673,10 +1673,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1687,10 +1687,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1701,10 +1701,10 @@
         <v>17</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1715,10 +1715,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1729,10 +1729,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1743,10 +1743,10 @@
         <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1757,10 +1757,10 @@
         <v>17</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1771,10 +1771,10 @@
         <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1785,10 +1785,10 @@
         <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1799,10 +1799,10 @@
         <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1813,10 +1813,10 @@
         <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1827,10 +1827,10 @@
         <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1841,10 +1841,10 @@
         <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1855,10 +1855,10 @@
         <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1869,10 +1869,10 @@
         <v>17</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1883,10 +1883,10 @@
         <v>17</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1897,7 +1897,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>31</v>
@@ -1911,10 +1911,10 @@
         <v>17</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1925,10 +1925,10 @@
         <v>17</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1939,10 +1939,10 @@
         <v>17</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1953,10 +1953,10 @@
         <v>17</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1967,10 +1967,10 @@
         <v>17</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1981,10 +1981,10 @@
         <v>17</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1995,10 +1995,10 @@
         <v>17</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2009,10 +2009,10 @@
         <v>17</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2023,10 +2023,10 @@
         <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2037,10 +2037,10 @@
         <v>17</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2051,10 +2051,10 @@
         <v>17</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2065,10 +2065,10 @@
         <v>17</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2079,10 +2079,10 @@
         <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2093,10 +2093,10 @@
         <v>17</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2107,10 +2107,10 @@
         <v>17</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2121,10 +2121,10 @@
         <v>17</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2135,10 +2135,10 @@
         <v>17</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2149,10 +2149,10 @@
         <v>17</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2163,10 +2163,10 @@
         <v>17</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2177,10 +2177,10 @@
         <v>17</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2191,10 +2191,10 @@
         <v>17</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2205,10 +2205,10 @@
         <v>17</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2219,10 +2219,10 @@
         <v>17</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2233,10 +2233,10 @@
         <v>17</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2247,10 +2247,10 @@
         <v>17</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2261,10 +2261,10 @@
         <v>17</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2275,10 +2275,10 @@
         <v>17</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2289,10 +2289,10 @@
         <v>17</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2303,10 +2303,10 @@
         <v>17</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2317,10 +2317,10 @@
         <v>17</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2331,10 +2331,10 @@
         <v>17</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2345,10 +2345,10 @@
         <v>17</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2359,10 +2359,10 @@
         <v>17</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -2373,10 +2373,10 @@
         <v>17</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L71" s="3"/>
       <c r="M71" s="6"/>
@@ -2389,16 +2389,16 @@
         <v>14</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>171</v>
+        <v>100</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="L72" s="3" t="s">
         <v>25</v>
@@ -2427,16 +2427,16 @@
         <v>14</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>25</v>
@@ -2465,16 +2465,16 @@
         <v>14</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F74" s="20" t="s">
-        <v>173</v>
+        <v>102</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="L74" s="3" t="s">
         <v>25</v>
@@ -2503,16 +2503,16 @@
         <v>14</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="L75" s="3" t="s">
         <v>25</v>
@@ -2541,16 +2541,16 @@
         <v>14</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>101</v>
+        <v>164</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>25</v>
@@ -2579,16 +2579,16 @@
         <v>14</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
       <c r="L77" s="3" t="s">
         <v>25</v>
@@ -2617,16 +2617,16 @@
         <v>14</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="L78" s="3" t="s">
         <v>25</v>
@@ -2655,16 +2655,16 @@
         <v>14</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="L79" s="3" t="s">
         <v>25</v>
@@ -2693,16 +2693,16 @@
         <v>14</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="L80" s="3" t="s">
         <v>25</v>
@@ -2731,16 +2731,16 @@
         <v>14</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>179</v>
+        <v>108</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>25</v>
@@ -2769,16 +2769,16 @@
         <v>14</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>25</v>
@@ -2807,16 +2807,16 @@
         <v>14</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>181</v>
+        <v>110</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>108</v>
+        <v>171</v>
       </c>
       <c r="L83" s="3" t="s">
         <v>25</v>
@@ -2845,16 +2845,16 @@
         <v>14</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>182</v>
+        <v>111</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="L84" s="3" t="s">
         <v>25</v>
@@ -2883,16 +2883,16 @@
         <v>14</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>183</v>
+        <v>112</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="L85" s="3" t="s">
         <v>25</v>
@@ -2921,16 +2921,16 @@
         <v>14</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="L86" s="3" t="s">
         <v>25</v>
@@ -2959,16 +2959,16 @@
         <v>14</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="L87" s="3" t="s">
         <v>25</v>
@@ -2997,16 +2997,16 @@
         <v>14</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="L88" s="3" t="s">
         <v>25</v>
@@ -3035,16 +3035,16 @@
         <v>14</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="L89" s="3" t="s">
         <v>25</v>
@@ -3073,16 +3073,16 @@
         <v>14</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>115</v>
+        <v>178</v>
       </c>
       <c r="L90" s="3" t="s">
         <v>25</v>
@@ -3111,16 +3111,16 @@
         <v>14</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>116</v>
+        <v>179</v>
       </c>
       <c r="L91" s="3" t="s">
         <v>25</v>
@@ -3149,16 +3149,16 @@
         <v>14</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="L92" s="3" t="s">
         <v>25</v>
@@ -3187,16 +3187,16 @@
         <v>14</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>118</v>
+        <v>181</v>
       </c>
       <c r="L93" s="3" t="s">
         <v>25</v>
@@ -3225,16 +3225,16 @@
         <v>14</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>119</v>
+        <v>182</v>
       </c>
       <c r="L94" s="3" t="s">
         <v>25</v>
@@ -3263,14 +3263,14 @@
         <v>14</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="2" t="s">
-        <v>120</v>
+        <v>183</v>
       </c>
       <c r="L95" s="3" t="s">
         <v>25</v>
@@ -3299,16 +3299,16 @@
         <v>14</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F96" s="19" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="L96" s="3" t="s">
         <v>25</v>
@@ -3337,16 +3337,16 @@
         <v>14</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F97" s="19" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>122</v>
+        <v>185</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>25</v>
@@ -3375,16 +3375,16 @@
         <v>14</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="L98" s="3" t="s">
         <v>25</v>
@@ -3413,16 +3413,16 @@
         <v>14</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="L99" s="3" t="s">
         <v>25</v>
@@ -3451,16 +3451,16 @@
         <v>14</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="L100" s="3" t="s">
         <v>25</v>
@@ -3489,16 +3489,16 @@
         <v>14</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="L101" s="3" t="s">
         <v>25</v>
@@ -3527,16 +3527,16 @@
         <v>14</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>127</v>
+        <v>190</v>
       </c>
       <c r="L102" s="3" t="s">
         <v>25</v>
@@ -3565,16 +3565,16 @@
         <v>14</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>128</v>
+        <v>191</v>
       </c>
       <c r="L103" s="3" t="s">
         <v>25</v>
@@ -3603,16 +3603,16 @@
         <v>14</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="L104" s="3" t="s">
         <v>25</v>
@@ -3641,16 +3641,16 @@
         <v>14</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>35</v>
+        <v>193</v>
       </c>
       <c r="L105" s="3" t="s">
         <v>25</v>
@@ -3679,16 +3679,16 @@
         <v>14</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>130</v>
+        <v>194</v>
       </c>
       <c r="L106" s="3" t="s">
         <v>25</v>
@@ -3717,16 +3717,16 @@
         <v>14</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>131</v>
+        <v>195</v>
       </c>
       <c r="L107" s="3" t="s">
         <v>25</v>
@@ -3755,16 +3755,16 @@
         <v>14</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F108" s="19" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>132</v>
+        <v>196</v>
       </c>
       <c r="L108" s="3" t="s">
         <v>25</v>
@@ -3793,16 +3793,16 @@
         <v>14</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F109" s="19" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
       <c r="L109" s="3" t="s">
         <v>25</v>
@@ -3831,16 +3831,16 @@
         <v>14</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="L110" s="3" t="s">
         <v>25</v>
@@ -3869,16 +3869,16 @@
         <v>14</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F111" s="19" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>135</v>
+        <v>199</v>
       </c>
       <c r="L111" s="3" t="s">
         <v>25</v>
@@ -3907,16 +3907,16 @@
         <v>14</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F112" s="19" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
       <c r="L112" s="3" t="s">
         <v>25</v>
@@ -3945,16 +3945,16 @@
         <v>14</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F113" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G113" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="L113" s="3" t="s">
         <v>25</v>
@@ -3983,16 +3983,16 @@
         <v>14</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F114" s="19" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="L114" s="3" t="s">
         <v>25</v>
@@ -4021,16 +4021,16 @@
         <v>14</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>25</v>
@@ -4059,16 +4059,16 @@
         <v>14</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="F116" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="L116" s="3" t="s">
         <v>25</v>
@@ -4097,16 +4097,16 @@
         <v>14</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="F117" s="20" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="L117" s="3" t="s">
         <v>25</v>
@@ -4135,16 +4135,16 @@
         <v>14</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="F118" s="19" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="L118" s="3" t="s">
         <v>25</v>
@@ -4173,16 +4173,16 @@
         <v>14</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
       <c r="F119" s="19" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="L119" s="3" t="s">
         <v>25</v>
@@ -4211,16 +4211,16 @@
         <v>14</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="L120" s="3" t="s">
         <v>25</v>
@@ -4249,16 +4249,16 @@
         <v>14</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F121" s="20" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="L121" s="3" t="s">
         <v>25</v>
@@ -4287,16 +4287,16 @@
         <v>14</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F122" s="19" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>139</v>
+        <v>210</v>
       </c>
       <c r="L122" s="3" t="s">
         <v>25</v>
@@ -4325,16 +4325,16 @@
         <v>14</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F123" s="19" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>140</v>
+        <v>211</v>
       </c>
       <c r="L123" s="3" t="s">
         <v>25</v>
@@ -4363,16 +4363,16 @@
         <v>14</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F124" s="19" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>141</v>
+        <v>212</v>
       </c>
       <c r="L124" s="3" t="s">
         <v>25</v>
@@ -4401,16 +4401,16 @@
         <v>14</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F125" s="19" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>142</v>
+        <v>213</v>
       </c>
       <c r="L125" s="3" t="s">
         <v>25</v>
@@ -4439,16 +4439,16 @@
         <v>14</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F126" s="20" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>143</v>
+        <v>214</v>
       </c>
       <c r="L126" s="3" t="s">
         <v>25</v>
@@ -4477,16 +4477,16 @@
         <v>14</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="L127" s="3" t="s">
         <v>25</v>
@@ -4515,16 +4515,16 @@
         <v>14</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>219</v>
+        <v>148</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>145</v>
+        <v>216</v>
       </c>
       <c r="L128" s="3" t="s">
         <v>25</v>
@@ -4553,16 +4553,16 @@
         <v>14</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>220</v>
+        <v>149</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>146</v>
+        <v>217</v>
       </c>
       <c r="L129" s="3" t="s">
         <v>25</v>
@@ -4591,16 +4591,16 @@
         <v>14</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F130" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>147</v>
+        <v>218</v>
       </c>
       <c r="L130" s="3" t="s">
         <v>25</v>
@@ -4629,16 +4629,16 @@
         <v>14</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F131" s="20" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="L131" s="3" t="s">
         <v>25</v>
@@ -4667,16 +4667,16 @@
         <v>14</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F132" s="19" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="L132" s="3" t="s">
         <v>25</v>
@@ -4705,16 +4705,16 @@
         <v>14</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F133" s="19" t="s">
-        <v>223</v>
+        <v>152</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="L133" s="3" t="s">
         <v>25</v>
@@ -4743,16 +4743,16 @@
         <v>14</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F134" s="19" t="s">
-        <v>224</v>
+        <v>153</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="L134" s="3" t="s">
         <v>25</v>
@@ -4781,16 +4781,16 @@
         <v>14</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F135" s="20" t="s">
-        <v>225</v>
+        <v>154</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="L135" s="3" t="s">
         <v>25</v>
@@ -4819,16 +4819,16 @@
         <v>14</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F136" s="19" t="s">
-        <v>226</v>
+        <v>155</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
       <c r="L136" s="3" t="s">
         <v>25</v>
@@ -4857,16 +4857,16 @@
         <v>14</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F137" s="19" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="L137" s="3" t="s">
         <v>25</v>
@@ -4895,16 +4895,16 @@
         <v>14</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="L138" s="3" t="s">
         <v>25</v>
@@ -4933,16 +4933,16 @@
         <v>14</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F139" s="19" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="L139" s="3" t="s">
         <v>25</v>
@@ -4992,17 +4992,17 @@
   </sheetData>
   <autoFilter ref="F72:G139" xr:uid="{0F4BE862-6320-9C46-8273-3C68143DBB4D}"/>
   <mergeCells count="11">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="V1:W1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>